<commit_message>
added info for elp1 ssbc
</commit_message>
<xml_diff>
--- a/cluster/analysis_elp1/metadata_elp1.xlsx
+++ b/cluster/analysis_elp1/metadata_elp1.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkinney/github/22_drugs/cluster/analysis_elp1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E39F9BC-6940-D342-8A4B-9D83D72BFC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="17625" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="30740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LIDs" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="119">
   <si>
     <t>LID</t>
   </si>
@@ -336,20 +341,56 @@
   </si>
   <si>
     <t>./cipher/cipher.ikbkap_rg_lib2_rep2_tot.txt</t>
+  </si>
+  <si>
+    <t>298871_S1_L001_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>298872_S2_L002_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>ikbkap_9nt_ssbc_lib1</t>
+  </si>
+  <si>
+    <t>ikbkap_9nt_ssbc_lib2</t>
+  </si>
+  <si>
+    <t>ikbkap_ssbc_read1</t>
+  </si>
+  <si>
+    <t>TTAATTAAAA.{86}AGTGGTTGGA(?P&lt;ss&gt;...G.....)GCCATTGTGC.*</t>
+  </si>
+  <si>
+    <t>TTAATTAAAAATGTTACTGCTTTAATTTATTTAAGATGCCAAGGGGAAACTTAGAAGTTGTTCATCATCGAGCCCTGGTTTTAGCTCAGATTCGGAAGTGGTTGGANNNGTNNNNGCCATTGTGCAGGTGGATGCACATGATGACATAAT</t>
+  </si>
+  <si>
+    <t>ikbkap_ssbc_read2</t>
+  </si>
+  <si>
+    <t>CTCGAG(?P&lt;bc_rc&gt;.{20})TCTAGAATGC.*</t>
+  </si>
+  <si>
+    <t>CTCGAGNNNNNNNNNNNNNNNNNNNNTCTAGAATGCAGGTGATTATGTCATCATGTGCATCCACCTGCACAATGGCNNNNACNNNTCCAACCACTTCCGAATCTGAGCTAAAACCAGGGCTCGATGATGAACAACTTCTAAGTTTCCCCT</t>
+  </si>
+  <si>
+    <t>298871_S1_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>298872_S2_L002_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>ss,bc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -360,386 +401,51 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Courier New"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -747,357 +453,86 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment shrinkToFit="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
-      <alignment shrinkToFit="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
-      <alignment shrinkToFit="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment shrinkToFit="true"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment shrinkToFit="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment shrinkToFit="true"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1221,7 +656,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1245,9 +680,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1271,7 +706,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1324,7 +759,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1349,247 +784,269 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMJ61"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="12" customWidth="true"/>
-    <col min="2" max="2" width="7" style="12" customWidth="true"/>
-    <col min="3" max="3" width="35.125" style="12" customWidth="true"/>
-    <col min="4" max="4" width="10.75" style="12" customWidth="true"/>
-    <col min="5" max="5" width="11.5083333333333" style="12" customWidth="true"/>
-    <col min="6" max="6" width="15.1333333333333" style="12" customWidth="true"/>
-    <col min="7" max="1024" width="9" style="12"/>
+    <col min="1" max="1" width="8.1640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="7" style="11" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="11" customWidth="1"/>
+    <col min="7" max="1024" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" s="17" customFormat="true" spans="1:6">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" s="17" customFormat="true" spans="1:6">
-      <c r="A2" s="12">
+    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23">
         <v>307750</v>
       </c>
-      <c r="B2" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="18">
         <v>44503</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" s="17" customFormat="true" spans="1:6">
-      <c r="A3" s="12">
+    <row r="3" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23">
         <v>307751</v>
       </c>
-      <c r="B3" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="18">
         <v>44503</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" s="17" customFormat="true" spans="1:6">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" s="17" customFormat="true" spans="1:6">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="15"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="18"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="15"/>
-      <c r="C9" s="15"/>
-    </row>
-    <row r="36" spans="3:3">
-      <c r="C36" s="15"/>
-    </row>
-    <row r="37" spans="3:3">
-      <c r="C37" s="15"/>
-    </row>
-    <row r="38" spans="3:3">
-      <c r="C38" s="15"/>
-    </row>
-    <row r="39" spans="3:3">
-      <c r="C39" s="15"/>
-    </row>
-    <row r="40" spans="3:3">
-      <c r="C40" s="15"/>
-    </row>
-    <row r="41" spans="3:3">
-      <c r="C41" s="15"/>
-    </row>
-    <row r="42" spans="3:3">
-      <c r="C42" s="15"/>
-    </row>
-    <row r="43" spans="3:3">
-      <c r="C43" s="15"/>
-    </row>
-    <row r="44" spans="3:3">
-      <c r="C44" s="15"/>
-    </row>
-    <row r="45" spans="3:3">
-      <c r="C45" s="15"/>
-    </row>
-    <row r="46" spans="3:3">
-      <c r="C46" s="15"/>
-    </row>
-    <row r="47" spans="3:3">
-      <c r="C47" s="15"/>
-    </row>
-    <row r="48" spans="3:3">
-      <c r="C48" s="15"/>
-    </row>
-    <row r="49" spans="3:3">
-      <c r="C49" s="15"/>
-    </row>
-    <row r="50" spans="3:3">
-      <c r="C50" s="15"/>
-    </row>
-    <row r="51" spans="3:3">
-      <c r="C51" s="15"/>
-    </row>
-    <row r="52" spans="3:3">
-      <c r="C52" s="15"/>
-    </row>
-    <row r="53" spans="3:3">
-      <c r="C53" s="15"/>
-    </row>
-    <row r="54" spans="3:3">
-      <c r="C54" s="15"/>
-    </row>
-    <row r="55" spans="3:3">
-      <c r="C55" s="15"/>
-    </row>
-    <row r="56" spans="3:3">
-      <c r="C56" s="15"/>
-    </row>
-    <row r="57" spans="3:3">
-      <c r="C57" s="15"/>
-    </row>
-    <row r="58" spans="3:3">
-      <c r="C58" s="15"/>
-    </row>
-    <row r="59" spans="3:3">
-      <c r="C59" s="15"/>
-    </row>
-    <row r="60" spans="3:3">
-      <c r="C60" s="15"/>
-    </row>
-    <row r="61" spans="3:3">
-      <c r="C61" s="15"/>
+    <row r="4" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="24">
+        <v>298871</v>
+      </c>
+      <c r="B4" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="18">
+        <v>42861</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="24">
+        <v>298872</v>
+      </c>
+      <c r="B5" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="18">
+        <v>42861</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="16"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="C9" s="13"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="13"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="13"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="13"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="13"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="13"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="13"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="13"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="13"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="13"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="13"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C48" s="13"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="13"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="13"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="13"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="13"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" s="13"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54" s="13"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55" s="13"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56" s="13"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" s="13"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58" s="13"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59" s="13"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60" s="13"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:I117"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMJ117"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.75" style="1" customWidth="true"/>
-    <col min="2" max="2" width="8.125" style="1" customWidth="true"/>
-    <col min="3" max="3" width="16.25" style="1" customWidth="true"/>
-    <col min="4" max="4" width="11.5" style="1" customWidth="true"/>
-    <col min="5" max="5" width="16.375" style="1" customWidth="true"/>
-    <col min="6" max="6" width="11.5083333333333" style="1" customWidth="true"/>
-    <col min="7" max="7" width="16.375" style="1" customWidth="true"/>
-    <col min="8" max="8" width="9.16666666666667" style="1" customWidth="true"/>
-    <col min="9" max="9" width="18.6666666666667" style="1" customWidth="true"/>
+    <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="1" customWidth="1"/>
     <col min="10" max="1024" width="9" style="1"/>
-    <col min="1025" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" spans="1:8">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1615,11 +1072,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" spans="1:8">
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>307750</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1637,15 +1094,15 @@
       <c r="G2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" s="3" customFormat="true" spans="1:8">
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>307750</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1663,15 +1120,15 @@
       <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" s="3" customFormat="true" spans="1:8">
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>307750</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1689,15 +1146,15 @@
       <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" s="3" customFormat="true" spans="1:8">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>307750</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1715,15 +1172,15 @@
       <c r="G5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" s="3" customFormat="true" spans="1:8">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>307750</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1741,15 +1198,15 @@
       <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="true" spans="1:8">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>307750</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1767,15 +1224,15 @@
       <c r="G7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="true" spans="1:8">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>307750</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1793,15 +1250,15 @@
       <c r="G8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="true" spans="1:8">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>307750</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1819,15 +1276,15 @@
       <c r="G9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="true" spans="1:8">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>307750</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1845,15 +1302,15 @@
       <c r="G10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" s="3" customFormat="true" spans="1:8">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>307750</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1871,15 +1328,15 @@
       <c r="G11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" s="3" customFormat="true" spans="1:8">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <v>307750</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1897,15 +1354,15 @@
       <c r="G12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" s="3" customFormat="true" spans="1:8">
+    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <v>307750</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1923,15 +1380,15 @@
       <c r="G13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="true" spans="1:8">
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <v>307751</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1949,15 +1406,15 @@
       <c r="G14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" s="3" customFormat="true" spans="1:8">
+    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <v>307751</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1975,15 +1432,15 @@
       <c r="G15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" s="3" customFormat="true" spans="1:8">
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>307751</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -2001,15 +1458,15 @@
       <c r="G16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" s="3" customFormat="true" spans="1:8">
+    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>307751</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2027,15 +1484,15 @@
       <c r="G17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" s="3" customFormat="true" spans="1:8">
+    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <v>307751</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -2053,15 +1510,15 @@
       <c r="G18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" s="3" customFormat="true" spans="1:8">
+    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="11">
         <v>307751</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -2079,15 +1536,15 @@
       <c r="G19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" s="3" customFormat="true" spans="1:8">
+    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="11">
         <v>307751</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -2105,15 +1562,15 @@
       <c r="G20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" s="3" customFormat="true" spans="1:8">
+    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="11">
         <v>307751</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -2131,15 +1588,15 @@
       <c r="G21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" s="3" customFormat="true" spans="1:8">
+    <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="11">
         <v>307751</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -2157,15 +1614,15 @@
       <c r="G22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" s="3" customFormat="true" spans="1:8">
+    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="11">
         <v>307751</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -2183,15 +1640,15 @@
       <c r="G23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" s="3" customFormat="true" spans="1:8">
+    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="11">
         <v>307751</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -2209,15 +1666,15 @@
       <c r="G24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" s="3" customFormat="true" spans="1:8">
+    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="11">
         <v>307751</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -2235,624 +1692,668 @@
       <c r="G25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" s="3" customFormat="true" spans="2:8">
-      <c r="B26" s="12"/>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" s="3" customFormat="true" spans="2:8">
-      <c r="B27" s="12"/>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" s="3" customFormat="true" spans="2:8">
-      <c r="B28" s="12"/>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" s="3" customFormat="true" spans="2:8">
-      <c r="B29" s="12"/>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="30" s="3" customFormat="true" spans="2:8">
-      <c r="B30" s="12"/>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" s="3" customFormat="true" spans="2:8">
-      <c r="B31" s="12"/>
-      <c r="H31" s="15"/>
-    </row>
-    <row r="32" s="3" customFormat="true" spans="2:8">
-      <c r="B32" s="12"/>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" s="3" customFormat="true" spans="2:8">
-      <c r="B33" s="12"/>
-      <c r="H33" s="15"/>
-    </row>
-    <row r="34" s="3" customFormat="true" spans="2:8">
-      <c r="B34" s="12"/>
-      <c r="H34" s="15"/>
-    </row>
-    <row r="35" s="3" customFormat="true" spans="2:8">
-      <c r="B35" s="12"/>
-      <c r="H35" s="15"/>
-    </row>
-    <row r="36" s="3" customFormat="true" spans="2:8">
-      <c r="B36" s="12"/>
-      <c r="H36" s="15"/>
-    </row>
-    <row r="37" s="3" customFormat="true" spans="2:8">
-      <c r="B37" s="12"/>
-      <c r="H37" s="15"/>
-    </row>
-    <row r="38" s="3" customFormat="true" spans="2:8">
-      <c r="B38" s="12"/>
-      <c r="H38" s="15"/>
-    </row>
-    <row r="39" s="3" customFormat="true" spans="2:8">
-      <c r="B39" s="12"/>
-      <c r="H39" s="15"/>
-    </row>
-    <row r="40" s="3" customFormat="true" spans="2:8">
-      <c r="B40" s="12"/>
-      <c r="H40" s="15"/>
-    </row>
-    <row r="41" s="3" customFormat="true" spans="2:8">
-      <c r="B41" s="12"/>
-      <c r="H41" s="15"/>
-    </row>
-    <row r="42" s="3" customFormat="true" spans="2:8">
-      <c r="B42" s="12"/>
-      <c r="H42" s="15"/>
-    </row>
-    <row r="43" s="3" customFormat="true" spans="2:8">
-      <c r="B43" s="12"/>
-      <c r="H43" s="15"/>
-    </row>
-    <row r="44" s="3" customFormat="true" spans="2:8">
-      <c r="B44" s="12"/>
-      <c r="H44" s="15"/>
-    </row>
-    <row r="45" s="3" customFormat="true" spans="2:8">
-      <c r="B45" s="12"/>
-      <c r="H45" s="15"/>
-    </row>
-    <row r="46" s="3" customFormat="true" spans="2:8">
-      <c r="B46" s="12"/>
-      <c r="H46" s="15"/>
-    </row>
-    <row r="47" s="3" customFormat="true" spans="2:8">
-      <c r="B47" s="12"/>
-      <c r="H47" s="15"/>
-    </row>
-    <row r="48" s="3" customFormat="true" spans="2:8">
-      <c r="B48" s="12"/>
-      <c r="H48" s="15"/>
-    </row>
-    <row r="49" s="3" customFormat="true" spans="2:8">
-      <c r="B49" s="12"/>
-      <c r="H49" s="15"/>
-    </row>
-    <row r="50" s="3" customFormat="true"/>
-    <row r="51" s="3" customFormat="true"/>
-    <row r="52" s="3" customFormat="true"/>
-    <row r="53" s="3" customFormat="true"/>
-    <row r="54" s="3" customFormat="true"/>
-    <row r="55" s="3" customFormat="true"/>
-    <row r="56" s="3" customFormat="true"/>
-    <row r="57" s="3" customFormat="true"/>
-    <row r="58" s="3" customFormat="true"/>
-    <row r="59" spans="1:7">
+    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="11">
+        <v>298871</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="11">
+        <v>298872</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="11"/>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="11"/>
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="11"/>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="11"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="11"/>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="11"/>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="11"/>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="11"/>
+      <c r="H35" s="13"/>
+    </row>
+    <row r="36" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="11"/>
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="11"/>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="11"/>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="11"/>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="11"/>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="11"/>
+      <c r="H41" s="13"/>
+    </row>
+    <row r="42" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="11"/>
+      <c r="H42" s="13"/>
+    </row>
+    <row r="43" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="11"/>
+      <c r="H43" s="13"/>
+    </row>
+    <row r="44" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="11"/>
+      <c r="H44" s="13"/>
+    </row>
+    <row r="45" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="11"/>
+      <c r="H45" s="13"/>
+    </row>
+    <row r="46" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="11"/>
+      <c r="H46" s="13"/>
+    </row>
+    <row r="47" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="11"/>
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="11"/>
+      <c r="H48" s="13"/>
+    </row>
+    <row r="49" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="11"/>
+      <c r="H49" s="13"/>
+    </row>
+    <row r="50" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="13"/>
+      <c r="D59" s="12"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="16"/>
+      <c r="F59" s="14"/>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="13"/>
+      <c r="D60" s="12"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="16"/>
+      <c r="F60" s="14"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="13"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="12"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="16"/>
+      <c r="F61" s="14"/>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="13"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="12"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="16"/>
+      <c r="F62" s="14"/>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="13"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="12"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="16"/>
+      <c r="F63" s="14"/>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="13"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="12"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="16"/>
+      <c r="F64" s="14"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="13"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="12"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="16"/>
+      <c r="F65" s="14"/>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="13"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="12"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="16"/>
+      <c r="F66" s="14"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="13"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="12"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="16"/>
+      <c r="F67" s="14"/>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="13"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="12"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="16"/>
+      <c r="F68" s="14"/>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="13"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="12"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="16"/>
+      <c r="F69" s="14"/>
       <c r="G69" s="3"/>
       <c r="I69" s="3"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="13"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="12"/>
       <c r="E70" s="3"/>
-      <c r="F70" s="16"/>
+      <c r="F70" s="14"/>
       <c r="G70" s="3"/>
       <c r="I70" s="3"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="13"/>
+      <c r="D71" s="12"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="16"/>
+      <c r="F71" s="14"/>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="13"/>
+      <c r="D72" s="12"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="16"/>
+      <c r="F72" s="14"/>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="13"/>
+      <c r="D73" s="12"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="16"/>
+      <c r="F73" s="14"/>
       <c r="G73" s="3"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="13"/>
+      <c r="D74" s="12"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="16"/>
+      <c r="F74" s="14"/>
       <c r="G74" s="3"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="13"/>
+      <c r="D75" s="12"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="16"/>
+      <c r="F75" s="14"/>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="13"/>
+      <c r="D76" s="12"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="16"/>
+      <c r="F76" s="14"/>
       <c r="G76" s="3"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="13"/>
+      <c r="D77" s="12"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="16"/>
+      <c r="F77" s="14"/>
       <c r="G77" s="3"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="13"/>
+      <c r="D78" s="12"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="16"/>
+      <c r="F78" s="14"/>
       <c r="G78" s="3"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="13"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="12"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="16"/>
+      <c r="F79" s="14"/>
       <c r="G79" s="3"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="13"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="12"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="16"/>
+      <c r="F80" s="14"/>
       <c r="G80" s="3"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="13"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="12"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="16"/>
+      <c r="F81" s="14"/>
       <c r="G81" s="3"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="13"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="12"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="16"/>
+      <c r="F82" s="14"/>
       <c r="G82" s="3"/>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="13"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="12"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="16"/>
+      <c r="F83" s="14"/>
       <c r="G83" s="3"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="13"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="12"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="16"/>
+      <c r="F84" s="14"/>
       <c r="G84" s="3"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="13"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="12"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="16"/>
+      <c r="F85" s="14"/>
       <c r="G85" s="3"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="13"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="12"/>
       <c r="E86" s="3"/>
-      <c r="F86" s="16"/>
+      <c r="F86" s="14"/>
       <c r="G86" s="3"/>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="13"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="12"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="16"/>
+      <c r="F87" s="14"/>
       <c r="G87" s="3"/>
       <c r="I87" s="3"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="13"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="12"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="16"/>
+      <c r="F88" s="14"/>
       <c r="G88" s="3"/>
       <c r="I88" s="3"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
-      <c r="D89" s="13"/>
+      <c r="D89" s="12"/>
       <c r="E89" s="3"/>
-      <c r="F89" s="16"/>
+      <c r="F89" s="14"/>
       <c r="G89" s="3"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
-      <c r="D90" s="13"/>
+      <c r="D90" s="12"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="16"/>
+      <c r="F90" s="14"/>
       <c r="G90" s="3"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
-      <c r="D91" s="13"/>
+      <c r="D91" s="12"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="16"/>
+      <c r="F91" s="14"/>
       <c r="G91" s="3"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
-      <c r="D92" s="13"/>
+      <c r="D92" s="12"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="16"/>
+      <c r="F92" s="14"/>
       <c r="G92" s="3"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
-      <c r="D93" s="13"/>
+      <c r="D93" s="12"/>
       <c r="E93" s="3"/>
-      <c r="F93" s="16"/>
+      <c r="F93" s="14"/>
       <c r="G93" s="3"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
-      <c r="D94" s="13"/>
+      <c r="D94" s="12"/>
       <c r="E94" s="3"/>
-      <c r="F94" s="16"/>
+      <c r="F94" s="14"/>
       <c r="G94" s="3"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
-      <c r="D95" s="13"/>
+      <c r="D95" s="12"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="16"/>
+      <c r="F95" s="14"/>
       <c r="G95" s="3"/>
       <c r="I95" s="3"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
-      <c r="D96" s="13"/>
+      <c r="D96" s="12"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="16"/>
+      <c r="F96" s="14"/>
       <c r="G96" s="3"/>
       <c r="I96" s="3"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
-      <c r="C97" s="14"/>
-      <c r="D97" s="13"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="12"/>
       <c r="E97" s="3"/>
-      <c r="F97" s="16"/>
+      <c r="F97" s="14"/>
       <c r="G97" s="3"/>
       <c r="I97" s="3"/>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
-      <c r="C98" s="14"/>
-      <c r="D98" s="13"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="12"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="16"/>
+      <c r="F98" s="14"/>
       <c r="G98" s="3"/>
       <c r="I98" s="3"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
-      <c r="C99" s="14"/>
-      <c r="D99" s="13"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="12"/>
       <c r="E99" s="3"/>
-      <c r="F99" s="16"/>
+      <c r="F99" s="14"/>
       <c r="G99" s="3"/>
       <c r="I99" s="3"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
-      <c r="C100" s="14"/>
-      <c r="D100" s="13"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="12"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="16"/>
+      <c r="F100" s="14"/>
       <c r="G100" s="3"/>
       <c r="I100" s="3"/>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
-      <c r="C101" s="14"/>
-      <c r="D101" s="13"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="12"/>
       <c r="E101" s="3"/>
-      <c r="F101" s="16"/>
+      <c r="F101" s="14"/>
       <c r="G101" s="3"/>
       <c r="I101" s="3"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
-      <c r="C102" s="14"/>
-      <c r="D102" s="13"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="12"/>
       <c r="E102" s="3"/>
-      <c r="F102" s="16"/>
+      <c r="F102" s="14"/>
       <c r="G102" s="3"/>
       <c r="I102" s="3"/>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
-      <c r="C103" s="14"/>
-      <c r="D103" s="13"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="12"/>
       <c r="E103" s="3"/>
-      <c r="F103" s="16"/>
+      <c r="F103" s="14"/>
       <c r="G103" s="3"/>
       <c r="I103" s="3"/>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
-      <c r="C104" s="14"/>
-      <c r="D104" s="13"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="12"/>
       <c r="E104" s="3"/>
-      <c r="F104" s="16"/>
+      <c r="F104" s="14"/>
       <c r="G104" s="3"/>
       <c r="I104" s="3"/>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
-      <c r="C105" s="14"/>
-      <c r="D105" s="13"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="12"/>
       <c r="E105" s="3"/>
-      <c r="F105" s="16"/>
+      <c r="F105" s="14"/>
       <c r="G105" s="3"/>
       <c r="I105" s="3"/>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
-      <c r="C106" s="14"/>
-      <c r="D106" s="13"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="12"/>
       <c r="E106" s="3"/>
-      <c r="F106" s="16"/>
+      <c r="F106" s="14"/>
       <c r="G106" s="3"/>
       <c r="I106" s="3"/>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
-      <c r="D107" s="13"/>
+      <c r="D107" s="12"/>
       <c r="E107" s="3"/>
-      <c r="F107" s="16"/>
+      <c r="F107" s="14"/>
       <c r="G107" s="3"/>
       <c r="I107" s="3"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
-      <c r="D108" s="13"/>
+      <c r="D108" s="12"/>
       <c r="E108" s="3"/>
-      <c r="F108" s="16"/>
+      <c r="F108" s="14"/>
       <c r="G108" s="3"/>
       <c r="I108" s="3"/>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
-      <c r="D109" s="13"/>
+      <c r="D109" s="12"/>
       <c r="E109" s="3"/>
-      <c r="F109" s="16"/>
+      <c r="F109" s="14"/>
       <c r="G109" s="3"/>
       <c r="I109" s="3"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
-      <c r="D110" s="13"/>
+      <c r="D110" s="12"/>
       <c r="E110" s="3"/>
-      <c r="F110" s="16"/>
+      <c r="F110" s="14"/>
       <c r="G110" s="3"/>
       <c r="I110" s="3"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
-      <c r="D111" s="13"/>
+      <c r="D111" s="12"/>
       <c r="E111" s="3"/>
-      <c r="F111" s="16"/>
+      <c r="F111" s="14"/>
       <c r="G111" s="3"/>
       <c r="I111" s="3"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
-      <c r="D112" s="13"/>
+      <c r="D112" s="12"/>
       <c r="E112" s="3"/>
-      <c r="F112" s="16"/>
+      <c r="F112" s="14"/>
       <c r="G112" s="3"/>
       <c r="I112" s="3"/>
     </row>
-    <row r="113" spans="4:9">
+    <row r="113" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
@@ -2860,7 +2361,7 @@
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
     </row>
-    <row r="114" spans="4:9">
+    <row r="114" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
@@ -2868,7 +2369,7 @@
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
     </row>
-    <row r="115" spans="4:9">
+    <row r="115" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
@@ -2876,7 +2377,7 @@
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
     </row>
-    <row r="116" spans="4:9">
+    <row r="116" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
@@ -2884,7 +2385,7 @@
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
     </row>
-    <row r="117" spans="4:9">
+    <row r="117" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
@@ -2893,30 +2394,28 @@
       <c r="I117" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+    <sheetView zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="1" customWidth="true"/>
-    <col min="2" max="2" width="61.5" style="1" customWidth="true"/>
-    <col min="3" max="3" width="209" style="1" customWidth="true"/>
+    <col min="1" max="1" width="17.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="209" style="1" customWidth="1"/>
     <col min="4" max="1024" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" spans="1:3">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -2927,7 +2426,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" ht="16.5" spans="1:4">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -2939,72 +2438,87 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="1:2">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="8"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="8"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="8"/>
     </row>
-    <row r="9" ht="16.5" spans="1:3">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="8"/>
       <c r="C9" s="10"/>
     </row>
-    <row r="10" ht="16.5" spans="1:3">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="8"/>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.5083333333333" style="1" customWidth="true"/>
-    <col min="2" max="2" width="13.8333333333333" style="1" customWidth="true"/>
-    <col min="3" max="3" width="50.125" style="1" customWidth="true"/>
+    <col min="1" max="1" width="35.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.1640625" style="1" customWidth="1"/>
     <col min="4" max="1024" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
@@ -3015,7 +2529,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>65</v>
       </c>
@@ -3026,7 +2540,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -3037,7 +2551,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>65</v>
       </c>
@@ -3048,7 +2562,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>72</v>
       </c>
@@ -3059,7 +2573,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
@@ -3070,7 +2584,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>72</v>
       </c>
@@ -3081,7 +2595,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>75</v>
       </c>
@@ -3092,7 +2606,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>75</v>
       </c>
@@ -3103,7 +2617,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>75</v>
       </c>
@@ -3114,7 +2628,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>79</v>
       </c>
@@ -3125,7 +2639,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>79</v>
       </c>
@@ -3136,7 +2650,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>79</v>
       </c>
@@ -3147,7 +2661,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>82</v>
       </c>
@@ -3158,7 +2672,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>82</v>
       </c>
@@ -3169,7 +2683,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>82</v>
       </c>
@@ -3180,7 +2694,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>85</v>
       </c>
@@ -3191,7 +2705,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>85</v>
       </c>
@@ -3202,7 +2716,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>85</v>
       </c>
@@ -3213,7 +2727,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>88</v>
       </c>
@@ -3224,7 +2738,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>88</v>
       </c>
@@ -3235,7 +2749,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>88</v>
       </c>
@@ -3246,7 +2760,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>91</v>
       </c>
@@ -3257,7 +2771,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>91</v>
       </c>
@@ -3268,7 +2782,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>91</v>
       </c>
@@ -3279,7 +2793,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>94</v>
       </c>
@@ -3290,7 +2804,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>94</v>
       </c>
@@ -3301,7 +2815,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>94</v>
       </c>
@@ -3312,7 +2826,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>97</v>
       </c>
@@ -3323,7 +2837,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>97</v>
       </c>
@@ -3334,7 +2848,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>97</v>
       </c>
@@ -3345,7 +2859,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>100</v>
       </c>
@@ -3356,7 +2870,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>100</v>
       </c>
@@ -3367,7 +2881,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>100</v>
       </c>
@@ -3378,7 +2892,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>103</v>
       </c>
@@ -3389,7 +2903,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>103</v>
       </c>
@@ -3400,7 +2914,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>103</v>
       </c>
@@ -3411,129 +2925,128 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="C59" s="3"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="C62" s="3"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="C65" s="3"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added ssbc fastq files to metadata_elp1.xlsx
</commit_message>
<xml_diff>
--- a/cluster/analysis_elp1/metadata_elp1.xlsx
+++ b/cluster/analysis_elp1/metadata_elp1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkinney/github/22_drugs/cluster/analysis_elp1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E39F9BC-6940-D342-8A4B-9D83D72BFC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B817D8ED-73FD-7D41-908B-FECDF6C01E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="30740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="27140" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LIDs" sheetId="1" r:id="rId1"/>
@@ -343,12 +343,6 @@
     <t>./cipher/cipher.ikbkap_rg_lib2_rep2_tot.txt</t>
   </si>
   <si>
-    <t>298871_S1_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>298872_S2_L002_R2_001.fastq.gz</t>
-  </si>
-  <si>
     <t>ikbkap_9nt_ssbc_lib1</t>
   </si>
   <si>
@@ -373,13 +367,19 @@
     <t>CTCGAGNNNNNNNNNNNNNNNNNNNNTCTAGAATGCAGGTGATTATGTCATCATGTGCATCCACCTGCACAATGGCNNNNACNNNTCCAACCACTTCCGAATCTGAGCTAAAACCAGGGCTCGATGATGAACAACTTCTAAGTTTCCCCT</t>
   </si>
   <si>
-    <t>298871_S1_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>298872_S2_L002_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>ss,bc</t>
+    <t>SRR6848167.sra_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>SRR6848167.sra_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>SRR6848170.sra_1.fastq.gz</t>
+  </si>
+  <si>
+    <t>SRR6848170.sra_2.fastq.gz</t>
+  </si>
+  <si>
+    <t>ss, bc</t>
   </si>
 </sst>
 </file>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,16 +881,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E4" s="18">
         <v>42861</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -901,16 +901,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>117</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>107</v>
       </c>
       <c r="E5" s="18">
         <v>42861</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1029,7 +1029,7 @@
   <dimension ref="A1:AMJ117"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B26" s="11">
         <v>298871</v>
@@ -1710,13 +1710,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F26" s="3" t="b">
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>118</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B27" s="11">
         <v>298872</v>
@@ -1736,13 +1736,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F27" s="3" t="b">
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H27" s="13" t="s">
         <v>118</v>
@@ -2440,24 +2440,24 @@
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2506,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>